<commit_message>
manual changes and other stuff
</commit_message>
<xml_diff>
--- a/Datasources/Austin_Home/austin_home_defensive_actions.xlsx
+++ b/Datasources/Austin_Home/austin_home_defensive_actions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossh\Projects\CITY_Soccer_Analysis\Datasources\Austin_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC31CD4C-E157-42BB-8062-32495AFA40C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744A23CB-2529-40F6-96EE-46C8CCA97F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Blocks</t>
   </si>
   <si>
-    <t>Unnamed: 21_level_0</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -88,24 +85,12 @@
     <t>Nicholas Gioacchini</t>
   </si>
   <si>
-    <t>Célio Pompeu</t>
-  </si>
-  <si>
     <t>Aziel Jackson</t>
   </si>
   <si>
-    <t>Tomáš Ostrák</t>
-  </si>
-  <si>
     <t>Jared Stroud</t>
   </si>
   <si>
-    <t>Nökkvi Þórisson</t>
-  </si>
-  <si>
-    <t>Eduard Löwen</t>
-  </si>
-  <si>
     <t>Njabulo Blom</t>
   </si>
   <si>
@@ -133,12 +118,6 @@
     <t>Joakim Nilsson</t>
   </si>
   <si>
-    <t>Roman Bürki</t>
-  </si>
-  <si>
-    <t>17 Players</t>
-  </si>
-  <si>
     <t>us USA</t>
   </si>
   <si>
@@ -256,10 +235,22 @@
     <t>Cha</t>
   </si>
   <si>
-    <t>Player ID</t>
-  </si>
-  <si>
     <t>Match ID</t>
+  </si>
+  <si>
+    <t>Celio Pompeu</t>
+  </si>
+  <si>
+    <t>Tomas Ostrak</t>
+  </si>
+  <si>
+    <t>Nokkvi Thorisson</t>
+  </si>
+  <si>
+    <t>Eduard Lowen</t>
+  </si>
+  <si>
+    <t>Roman Burki</t>
   </si>
 </sst>
 </file>
@@ -628,207 +619,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>1</v>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2">
+        <v>80</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>20</v>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>24</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="D4">
-        <v>11</v>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="G4">
+        <v>86</v>
       </c>
       <c r="H4">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -843,45 +902,42 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V4">
         <v>0</v>
       </c>
       <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>24</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -928,58 +984,55 @@
       <c r="W5">
         <v>0</v>
       </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>24</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="G6">
+        <v>80</v>
       </c>
       <c r="H6">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>2</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -994,42 +1047,39 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>0</v>
       </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>24</v>
       </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1038,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1056,19 +1106,19 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T7">
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -1076,40 +1126,37 @@
       <c r="W7">
         <v>0</v>
       </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>24</v>
       </c>
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="G8">
+        <v>90</v>
       </c>
       <c r="H8">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1118,13 +1165,13 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1133,16 +1180,16 @@
         <v>2</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1150,117 +1197,111 @@
       <c r="W8">
         <v>0</v>
       </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>24</v>
       </c>
-      <c r="B9" s="1">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9">
-        <v>29</v>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9">
         <v>64</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9">
         <v>0</v>
       </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>24</v>
       </c>
-      <c r="B10" s="1">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>26</v>
       </c>
       <c r="H10">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1272,19 +1313,19 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -1293,48 +1334,45 @@
         <v>1</v>
       </c>
       <c r="V10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>24</v>
       </c>
-      <c r="B11" s="1">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G11">
+        <v>64</v>
       </c>
       <c r="H11">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1343,69 +1381,66 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q11">
         <v>2</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>24</v>
       </c>
-      <c r="B12" s="1">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>19</v>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="G12">
+        <v>26</v>
       </c>
       <c r="H12">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1414,19 +1449,19 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1435,10 +1470,10 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V12">
         <v>1</v>
@@ -1446,40 +1481,37 @@
       <c r="W12">
         <v>0</v>
       </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>24</v>
       </c>
-      <c r="B13" s="1">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>21</v>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>90</v>
       </c>
       <c r="H13">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1494,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1506,51 +1538,48 @@
         <v>2</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>24</v>
       </c>
-      <c r="B14" s="1">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14">
-        <v>16</v>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="G14">
+        <v>90</v>
       </c>
       <c r="H14">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1559,90 +1588,87 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W14">
-        <v>1</v>
-      </c>
-      <c r="X14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>24</v>
       </c>
-      <c r="B15" s="1">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15">
-        <v>22</v>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" t="s">
-        <v>70</v>
+        <v>65</v>
+      </c>
+      <c r="G15">
+        <v>90</v>
       </c>
       <c r="H15">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1651,81 +1677,78 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>1</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W15">
-        <v>3</v>
-      </c>
-      <c r="X15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>24</v>
       </c>
-      <c r="B16" s="1">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16">
-        <v>26</v>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G16">
+        <v>86</v>
       </c>
       <c r="H16">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>66.7</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -1734,48 +1757,45 @@
         <v>1</v>
       </c>
       <c r="U16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V16">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W16">
-        <v>4</v>
-      </c>
-      <c r="X16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>24</v>
       </c>
-      <c r="B17" s="1">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
       </c>
       <c r="H17">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1784,22 +1804,22 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -1808,69 +1828,66 @@
         <v>0</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>4</v>
-      </c>
-      <c r="X17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>24</v>
       </c>
-      <c r="B18" s="1">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18">
-        <v>20</v>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="G18">
+        <v>90</v>
       </c>
       <c r="H18">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>66.7</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1882,225 +1899,12 @@
         <v>0</v>
       </c>
       <c r="U18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>7</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>24</v>
-      </c>
-      <c r="B19" s="1">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19">
-        <v>4</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>2</v>
-      </c>
-      <c r="S19">
-        <v>2</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20">
-        <v>90</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21">
-        <v>990</v>
-      </c>
-      <c r="I21">
-        <v>15</v>
-      </c>
-      <c r="J21">
-        <v>7</v>
-      </c>
-      <c r="K21">
-        <v>9</v>
-      </c>
-      <c r="L21">
-        <v>4</v>
-      </c>
-      <c r="M21">
-        <v>2</v>
-      </c>
-      <c r="N21">
-        <v>7</v>
-      </c>
-      <c r="O21">
-        <v>16</v>
-      </c>
-      <c r="P21">
-        <v>43.8</v>
-      </c>
-      <c r="Q21">
-        <v>9</v>
-      </c>
-      <c r="R21">
-        <v>13</v>
-      </c>
-      <c r="S21">
-        <v>6</v>
-      </c>
-      <c r="T21">
-        <v>7</v>
-      </c>
-      <c r="U21">
-        <v>7</v>
-      </c>
-      <c r="V21">
-        <v>22</v>
-      </c>
-      <c r="W21">
-        <v>20</v>
-      </c>
-      <c r="X21">
         <v>0</v>
       </c>
     </row>

</xml_diff>